<commit_message>
flexible first elimination round
</commit_message>
<xml_diff>
--- a/tournaments/2024-mens-copa-america.xlsx
+++ b/tournaments/2024-mens-copa-america.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruceo\Documents\code\soccer-tourney-poster\tournaments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B584237-A6C8-440F-B706-AEE9687A13D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE780750-98F8-48E3-ABD5-843F35083EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1467" yWindow="1467" windowWidth="19200" windowHeight="10073" activeTab="3" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
+    <workbookView xWindow="2567" yWindow="2567" windowWidth="19200" windowHeight="10073" activeTab="1" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tournament" sheetId="8" r:id="rId1"/>
@@ -593,9 +593,6 @@
     <t>W29</t>
   </si>
   <si>
-    <t>W39</t>
-  </si>
-  <si>
     <t>#b0d0ee</t>
   </si>
   <si>
@@ -606,6 +603,9 @@
   </si>
   <si>
     <t>#fee289</t>
+  </si>
+  <si>
+    <t>W30</t>
   </si>
 </sst>
 </file>
@@ -1609,8 +1609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ABE575-0207-4299-82CD-74F27B6194DA}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2316,7 +2316,7 @@
         <v>183</v>
       </c>
       <c r="C33" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="D33" s="1">
         <v>45488</v>
@@ -2498,7 +2498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE2E615E-FE08-4442-901C-E33FB48A622A}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2541,10 +2541,10 @@
         <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.5">
@@ -2563,7 +2563,7 @@
         <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J4" t="s">
         <v>73</v>
@@ -2574,7 +2574,7 @@
         <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J5" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
corrected copa america schedule/matchups
</commit_message>
<xml_diff>
--- a/tournaments/2024-mens-copa-america.xlsx
+++ b/tournaments/2024-mens-copa-america.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruceo\Documents\code\soccer-tourney-poster\tournaments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE780750-98F8-48E3-ABD5-843F35083EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95DEA38-39F4-4704-90AB-9635FEEF41B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2567" yWindow="2567" windowWidth="19200" windowHeight="10073" activeTab="1" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="1" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tournament" sheetId="8" r:id="rId1"/>
@@ -707,6 +707,9 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D36B1D81-AA68-4E33-AA36-B206B4FF7406}" name="matches" displayName="matches" ref="A1:K33" totalsRowShown="0">
   <autoFilter ref="A1:K33" xr:uid="{D36B1D81-AA68-4E33-AA36-B206B4FF7406}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K33">
+    <sortCondition ref="A1:A33"/>
+  </sortState>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{35D3E9F5-BB3B-4940-9EB6-C927FD84875C}" name="match"/>
     <tableColumn id="2" xr3:uid="{97337EE3-AAC3-4452-8381-1A56C6B35138}" name="home-seed"/>
@@ -1610,7 +1613,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -1689,7 +1692,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="1">
-        <v>45465.041666666672</v>
+        <v>45465</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1704,16 +1707,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1">
-        <v>45466.041666666664</v>
+        <v>45466.041666666672</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -1725,16 +1728,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1">
-        <v>45466</v>
+        <v>45465.916666666664</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1752,7 +1755,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="1">
-        <v>45466.958333333336</v>
+        <v>45466.916666666672</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -1773,7 +1776,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="1">
-        <v>45466.958333333328</v>
+        <v>45467.041666666664</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -1788,16 +1791,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1">
-        <v>45467.958333333336</v>
+        <v>45468.041666666664</v>
       </c>
       <c r="E8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1809,16 +1812,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="1">
-        <v>45468.083333333328</v>
+        <v>45467.916666666672</v>
       </c>
       <c r="E9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1830,16 +1833,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D10" s="1">
-        <v>45468.958333333336</v>
+        <v>45469.041666666664</v>
       </c>
       <c r="E10">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1851,16 +1854,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1">
-        <v>45469.041666666664</v>
+        <v>45468.916666666672</v>
       </c>
       <c r="E11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1872,16 +1875,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D12" s="1">
         <v>45470.041666666664</v>
       </c>
       <c r="E12">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1893,16 +1896,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D13" s="1">
-        <v>45470.083333333328</v>
+        <v>45469.916666666664</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1941,7 +1944,7 @@
         <v>13</v>
       </c>
       <c r="D15" s="1">
-        <v>45470.958333333328</v>
+        <v>45471.041666666664</v>
       </c>
       <c r="E15">
         <v>8</v>
@@ -1956,16 +1959,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D16" s="1">
         <v>45472.041666666664</v>
       </c>
       <c r="E16">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -1977,16 +1980,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="1">
+        <v>45471.916666666664</v>
+      </c>
+      <c r="E17">
         <v>10</v>
-      </c>
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="1">
-        <v>45472.083333333328</v>
-      </c>
-      <c r="E17">
-        <v>9</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -2040,16 +2043,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D20" s="1">
-        <v>45474.041666666672</v>
+        <v>45474</v>
       </c>
       <c r="E20">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -2061,16 +2064,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D21" s="1">
-        <v>45474.125</v>
+        <v>45474</v>
       </c>
       <c r="E21">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -2082,16 +2085,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="1">
+        <v>45475.041666666672</v>
+      </c>
+      <c r="E22">
         <v>13</v>
-      </c>
-      <c r="C22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="1">
-        <v>45475.041666666664</v>
-      </c>
-      <c r="E22">
-        <v>11</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -2103,16 +2106,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D23" s="1">
-        <v>45475.083333333336</v>
+        <v>45475.041666666664</v>
       </c>
       <c r="E23">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -2124,16 +2127,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D24" s="1">
-        <v>45476.083333333336</v>
+        <v>45476.041666666664</v>
       </c>
       <c r="E24">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -2145,16 +2148,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D25" s="1">
-        <v>45476.166666666664</v>
+        <v>45476.041666666672</v>
       </c>
       <c r="E25">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -2277,7 +2280,7 @@
         <v>180</v>
       </c>
       <c r="D31" s="1">
-        <v>45483</v>
+        <v>45484</v>
       </c>
       <c r="E31">
         <v>14</v>

</xml_diff>

<commit_message>
scratch sheets start with '#'... move them from "work" books
</commit_message>
<xml_diff>
--- a/tournaments/2024-mens-copa-america.xlsx
+++ b/tournaments/2024-mens-copa-america.xlsx
@@ -8,15 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruceo\Documents\code\soccer-tourney-poster\tournaments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95DEA38-39F4-4704-90AB-9635FEEF41B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD0B3EF-B5B4-49C9-AA6F-949030B48964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="1" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="8" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tournament" sheetId="8" r:id="rId1"/>
     <sheet name="Matches" sheetId="1" r:id="rId2"/>
     <sheet name="Seeds" sheetId="3" r:id="rId3"/>
     <sheet name="Colors" sheetId="9" r:id="rId4"/>
+    <sheet name="#matches" sheetId="10" r:id="rId5"/>
+    <sheet name="#seeds" sheetId="11" r:id="rId6"/>
+    <sheet name="#teams" sheetId="12" r:id="rId7"/>
+    <sheet name="#venues" sheetId="13" r:id="rId8"/>
+    <sheet name="#cities" sheetId="14" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,8 +43,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="405">
   <si>
     <t>A1</t>
   </si>
@@ -606,16 +633,666 @@
   </si>
   <si>
     <t>W30</t>
+  </si>
+  <si>
+    <t>Miami, FL (Hard Rock Stadium)</t>
+  </si>
+  <si>
+    <t>Match 30 Winner</t>
+  </si>
+  <si>
+    <t>Match 29 Winner</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Charlotte, NC (Bank of America Stadium)</t>
+  </si>
+  <si>
+    <t>Match 30 Loser</t>
+  </si>
+  <si>
+    <t>Match 29 Loser</t>
+  </si>
+  <si>
+    <t>Third</t>
+  </si>
+  <si>
+    <t>Match 28 Winner</t>
+  </si>
+  <si>
+    <t>Match 27 Winner</t>
+  </si>
+  <si>
+    <t>East Rutherford, NJ (MetLife Stadium)</t>
+  </si>
+  <si>
+    <t>Match 26 Winner</t>
+  </si>
+  <si>
+    <t>Match 25 Winner</t>
+  </si>
+  <si>
+    <t>Semis</t>
+  </si>
+  <si>
+    <t>Glendale, AZ (State Farm Stadium)</t>
+  </si>
+  <si>
+    <t>Group C Runner Up</t>
+  </si>
+  <si>
+    <t>Group D Winner</t>
+  </si>
+  <si>
+    <t>Las Vegas, NV (Allegiant Stadium)</t>
+  </si>
+  <si>
+    <t>Group D Runner Up</t>
+  </si>
+  <si>
+    <t>Group C Winner</t>
+  </si>
+  <si>
+    <t>Arlington, TX (AT&amp;T Stadium)</t>
+  </si>
+  <si>
+    <t>Group A Runner Up</t>
+  </si>
+  <si>
+    <t>Group B Winner</t>
+  </si>
+  <si>
+    <t>Houston, TX (NRG Stadium)</t>
+  </si>
+  <si>
+    <t>Group B Runner Up</t>
+  </si>
+  <si>
+    <t>Group A Winner</t>
+  </si>
+  <si>
+    <t>Quarters</t>
+  </si>
+  <si>
+    <t>Austin, TX (Q2 Stadium)</t>
+  </si>
+  <si>
+    <t>Paraguay</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>Santa Clara, CA (Levi's Stadium)</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Orlando, FL (Exploria Stadium)</t>
+  </si>
+  <si>
+    <t>Panama</t>
+  </si>
+  <si>
+    <t>Bolivia</t>
+  </si>
+  <si>
+    <t>Kansas City, MO (Arrowhead Stadium)</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
+  </si>
+  <si>
+    <t>Jamaica</t>
+  </si>
+  <si>
+    <t>Ecuador</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Peru</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Atlanta, GA (Mercedes-Benz Stadium)</t>
+  </si>
+  <si>
+    <t>Inglewood, CA (SoFi Stadium)</t>
+  </si>
+  <si>
+    <t>Kansas City, KS (Children's Mercy Park)</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>date.utc</t>
+  </si>
+  <si>
+    <t>away.seed</t>
+  </si>
+  <si>
+    <t>home.seed</t>
+  </si>
+  <si>
+    <t>away.code</t>
+  </si>
+  <si>
+    <t>home.code</t>
+  </si>
+  <si>
+    <t>location.tz</t>
+  </si>
+  <si>
+    <t>location.code</t>
+  </si>
+  <si>
+    <t>away</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>team.lower</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>zam</t>
+  </si>
+  <si>
+    <t>Wales</t>
+  </si>
+  <si>
+    <t>wal</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>vie</t>
+  </si>
+  <si>
+    <t>ven</t>
+  </si>
+  <si>
+    <t>usa</t>
+  </si>
+  <si>
+    <t>uru</t>
+  </si>
+  <si>
+    <t>Un. Ar. Emirates</t>
+  </si>
+  <si>
+    <t>uae</t>
+  </si>
+  <si>
+    <t>Ukraine</t>
+  </si>
+  <si>
+    <t>ukr</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>tur</t>
+  </si>
+  <si>
+    <t>Tunisia</t>
+  </si>
+  <si>
+    <t>tun</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>sui</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>swe</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>esp</t>
+  </si>
+  <si>
+    <t>South Korea</t>
+  </si>
+  <si>
+    <t>kor</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>saf</t>
+  </si>
+  <si>
+    <t>Slovenia</t>
+  </si>
+  <si>
+    <t>svn</t>
+  </si>
+  <si>
+    <t>Slovakia</t>
+  </si>
+  <si>
+    <t>svk</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
+    <t>srb</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>sen</t>
+  </si>
+  <si>
+    <t>Scotland</t>
+  </si>
+  <si>
+    <t>sco</t>
+  </si>
+  <si>
+    <t>Saudi Arabia</t>
+  </si>
+  <si>
+    <t>ksa</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>rus</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>rom</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>qat</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>por</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>pol</t>
+  </si>
+  <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>phi</t>
+  </si>
+  <si>
+    <t>per</t>
+  </si>
+  <si>
+    <t>par</t>
+  </si>
+  <si>
+    <t>pan</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>nor</t>
+  </si>
+  <si>
+    <t>Northern Ireland</t>
+  </si>
+  <si>
+    <t>nir</t>
+  </si>
+  <si>
+    <t>North Macedonia</t>
+  </si>
+  <si>
+    <t>nmc</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>nga</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>nzl</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>ned</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>mar</t>
+  </si>
+  <si>
+    <t>Montenegro</t>
+  </si>
+  <si>
+    <t>mon</t>
+  </si>
+  <si>
+    <t>mex</t>
+  </si>
+  <si>
+    <t>Mali</t>
+  </si>
+  <si>
+    <t>mal</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>jpn</t>
+  </si>
+  <si>
+    <t>jam</t>
+  </si>
+  <si>
+    <t>Ivory Coast</t>
+  </si>
+  <si>
+    <t>ivc</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>ita</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>isr</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>ire</t>
+  </si>
+  <si>
+    <t>Iraq</t>
+  </si>
+  <si>
+    <t>irq</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>irn</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>isl</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>hun</t>
+  </si>
+  <si>
+    <t>Honduras</t>
+  </si>
+  <si>
+    <t>hon</t>
+  </si>
+  <si>
+    <t>Haiti</t>
+  </si>
+  <si>
+    <t>hai</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>gre</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>gha</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>ger</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>geo</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>fra</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>fin</t>
+  </si>
+  <si>
+    <t>England</t>
+  </si>
+  <si>
+    <t>eng</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>egy</t>
+  </si>
+  <si>
+    <t>ecu</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>den</t>
+  </si>
+  <si>
+    <t>Czechia</t>
+  </si>
+  <si>
+    <t>cze</t>
+  </si>
+  <si>
+    <t>Croatia</t>
+  </si>
+  <si>
+    <t>cro</t>
+  </si>
+  <si>
+    <t>crc</t>
+  </si>
+  <si>
+    <t>Congo</t>
+  </si>
+  <si>
+    <t>con</t>
+  </si>
+  <si>
+    <t>col</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>chi</t>
+  </si>
+  <si>
+    <t>can</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
+    <t>cmr</t>
+  </si>
+  <si>
+    <t>Burkina Faso</t>
+  </si>
+  <si>
+    <t>bfs</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>bul</t>
+  </si>
+  <si>
+    <t>bra</t>
+  </si>
+  <si>
+    <t>Bosnia a. Herzeg.</t>
+  </si>
+  <si>
+    <t>bah</t>
+  </si>
+  <si>
+    <t>bol</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>bel</t>
+  </si>
+  <si>
+    <t>Belarus</t>
+  </si>
+  <si>
+    <t>blr</t>
+  </si>
+  <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>aut</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>aus</t>
+  </si>
+  <si>
+    <t>Armenia</t>
+  </si>
+  <si>
+    <t>arm</t>
+  </si>
+  <si>
+    <t>arg</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>alg</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>alb</t>
+  </si>
+  <si>
+    <t>tz</t>
+  </si>
+  <si>
+    <t>city</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="165" formatCode="h:mm;@"/>
+    <numFmt numFmtId="166" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -629,16 +1306,80 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -646,18 +1387,545 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="8" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="18" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="18" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="35">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="23" formatCode="h:mm\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="h:mm;@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="m/d/yy\ h:mm;@"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
     </dxf>
@@ -715,13 +1983,13 @@
     <tableColumn id="2" xr3:uid="{97337EE3-AAC3-4452-8381-1A56C6B35138}" name="home-seed"/>
     <tableColumn id="3" xr3:uid="{AEDB8750-5B25-4357-9054-E49FECC94717}" name="away-seed"/>
     <tableColumn id="4" xr3:uid="{B178F43D-E631-4314-9E59-2CDA6EDA94F1}" name="time"/>
-    <tableColumn id="5" xr3:uid="{A42548B2-C8DF-4D47-B798-8E23FCB67696}" name="venue" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{A42548B2-C8DF-4D47-B798-8E23FCB67696}" name="venue" dataDxfId="34"/>
     <tableColumn id="11" xr3:uid="{FC876643-4BF9-4FDA-A0ED-DF50FF384B1F}" name="home-team"/>
     <tableColumn id="10" xr3:uid="{E5D59926-7D0A-4689-A049-F55DB0E286E9}" name="away-team"/>
-    <tableColumn id="6" xr3:uid="{A0CDBBB6-1128-45BC-8300-89FE399860C1}" name="home-score" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{95DA1082-F87D-4A64-B45A-77AEEA888386}" name="away-score" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{5865175D-2339-4B50-A707-595597D0BEF5}" name="home-tiebreaker" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{967E27DF-151D-40C4-9623-59691A5D7311}" name="away-tiebreaker" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{A0CDBBB6-1128-45BC-8300-89FE399860C1}" name="home-score" dataDxfId="33"/>
+    <tableColumn id="9" xr3:uid="{95DA1082-F87D-4A64-B45A-77AEEA888386}" name="away-score" dataDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{5865175D-2339-4B50-A707-595597D0BEF5}" name="home-tiebreaker" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{967E27DF-151D-40C4-9623-59691A5D7311}" name="away-tiebreaker" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -752,6 +2020,71 @@
     <tableColumn id="8" xr3:uid="{373F278C-AA56-4847-9936-7CDB1D93754B}" name="ja"/>
     <tableColumn id="9" xr3:uid="{6DCFFACA-53BA-4D49-9A7E-5B9205135116}" name="fa"/>
     <tableColumn id="10" xr3:uid="{5B623E17-AB69-4899-927D-0EBF9050D049}" name="notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9CE04D0A-CAC9-42EF-999D-5A90EB55AC28}" name="Table3" displayName="Table3" ref="A1:M33" totalsRowShown="0" headerRowDxfId="15" tableBorderDxfId="29">
+  <autoFilter ref="A1:M33" xr:uid="{9CE04D0A-CAC9-42EF-999D-5A90EB55AC28}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{1B8255EA-385E-448C-BFF0-15D3FAEB008C}" name="match" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{333537F6-02DC-43D1-AE95-2FDA8F8545AE}" name="group" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{A623E5AF-6F77-48E7-8408-C9DF33B599FE}" name="date" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{C71C8116-A80F-4C88-94D2-2105510B6845}" name="home" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{360B7BF3-162A-4D2D-9DBF-E6AD730C2F1C}" name="away" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{58920BD6-62A5-4370-9E66-99B922B1F84A}" name="location" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{D8DE90CC-C321-4A0F-9631-FFBAB5E0C1DD}" name="location.code" dataDxfId="22">
+      <calculatedColumnFormula>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F2,'#venues'!$B$2:$B$15,0))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{479E0FC3-8C44-42F5-91D0-CAF341856CFF}" name="location.tz" dataDxfId="21">
+      <calculatedColumnFormula>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F2,'#venues'!$B$2:$B$15,0))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{33B555FF-1525-4647-8A26-4AF178C2D50B}" name="home.code" dataDxfId="20"/>
+    <tableColumn id="10" xr3:uid="{6F01F904-7CD0-4562-9012-AAD0625BAC1F}" name="away.code" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{C5F18400-9B55-416A-9A39-94E52CE8614C}" name="home.seed" dataDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{BBE9B22F-B8EB-4D6D-ACF4-D15933365443}" name="away.seed" dataDxfId="17"/>
+    <tableColumn id="13" xr3:uid="{0B3917F1-1F81-4F48-BF79-07CD54D45594}" name="date.utc" dataDxfId="16">
+      <calculatedColumnFormula>'#matches'!$C2+'#matches'!$H2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9D892A45-FE66-44EC-8988-5C861DD34C69}" name="Table5" displayName="Table5" ref="A1:C17" totalsRowShown="0" headerRowDxfId="10" tableBorderDxfId="14">
+  <autoFilter ref="A1:C17" xr:uid="{9D892A45-FE66-44EC-8988-5C861DD34C69}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{C1EB50F5-D1BA-4A80-98D6-4FD530839378}" name="seed" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{2F8DD596-1F8D-4A24-96B9-1556EF0599C0}" name="team" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{FD8E5E2E-FCE0-4D70-A055-845C6FE30B08}" name="team.lower" dataDxfId="11">
+      <calculatedColumnFormula>LOWER('#seeds'!$B2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{04A99FB6-88C7-4CB5-8839-ECB08BD14B01}" name="Table6" displayName="Table6" ref="A1:B86" totalsRowShown="0" headerRowDxfId="5" dataDxfId="6" tableBorderDxfId="9">
+  <autoFilter ref="A1:B86" xr:uid="{04A99FB6-88C7-4CB5-8839-ECB08BD14B01}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{4BA3BBA0-E012-47FE-A8C1-BE58E18A5252}" name="key" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{CFF7F808-07C8-489E-A17F-2EA1332F910D}" name="en" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{F21910B9-B0EE-4804-8298-B1FEC2574266}" name="Table8" displayName="Table8" ref="A1:C15" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="4">
+  <autoFilter ref="A1:C15" xr:uid="{F21910B9-B0EE-4804-8298-B1FEC2574266}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{3067016A-DAE9-4C32-B681-2121ED9ADBFD}" name="venue" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{9EE6702F-E7B5-441A-A332-F6944F8C7751}" name="city" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{FFC8A035-989F-4D69-A3E9-A49C55C8AB96}" name="tz" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1612,7 +2945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ABE575-0207-4299-82CD-74F27B6194DA}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
@@ -2590,4 +3923,2962 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCC56A64-9C14-42A9-A137-A87AB9C697B6}">
+  <dimension ref="A1:M33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:M33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.7" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="3" max="3" width="12.52734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.76171875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.64453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5859375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="20.9375" customWidth="1"/>
+    <col min="9" max="9" width="11.703125" customWidth="1"/>
+    <col min="10" max="10" width="11.29296875" customWidth="1"/>
+    <col min="11" max="11" width="11.5859375" customWidth="1"/>
+    <col min="12" max="12" width="11.17578125" customWidth="1"/>
+    <col min="13" max="13" width="20.3515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A1" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="I1" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="4">
+        <v>45463.833333333336</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="G2" s="2">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F2,'#venues'!$B$2:$B$15,0))</f>
+        <v>1</v>
+      </c>
+      <c r="H2" s="3">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F2,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I2" s="2" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$D2,'#teams'!$B$2:$B$86,0))</f>
+        <v>arg</v>
+      </c>
+      <c r="J2" s="2" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$E2,'#teams'!$B$2:$B$86,0))</f>
+        <v>can</v>
+      </c>
+      <c r="K2" s="2" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$I2,'#seeds'!$C$2:$C$17,0))</f>
+        <v>A1</v>
+      </c>
+      <c r="L2" s="2" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$J2,'#seeds'!$C$2:$C$17,0))</f>
+        <v>A4</v>
+      </c>
+      <c r="M2" s="18">
+        <f>'#matches'!$C2+'#matches'!$H2</f>
+        <v>45464</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="7">
+        <v>45464.791666666664</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="G3" s="5">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F3,'#venues'!$B$2:$B$15,0))</f>
+        <v>2</v>
+      </c>
+      <c r="H3" s="6">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F3,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="I3" s="5" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$D3,'#teams'!$B$2:$B$86,0))</f>
+        <v>per</v>
+      </c>
+      <c r="J3" s="5" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$E3,'#teams'!$B$2:$B$86,0))</f>
+        <v>chi</v>
+      </c>
+      <c r="K3" s="5" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$I3,'#seeds'!$C$2:$C$17,0))</f>
+        <v>A2</v>
+      </c>
+      <c r="L3" s="5" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$J3,'#seeds'!$C$2:$C$17,0))</f>
+        <v>A3</v>
+      </c>
+      <c r="M3" s="19">
+        <f>'#matches'!$C3+'#matches'!$H3</f>
+        <v>45465</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="4">
+        <v>45465.833333333336</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G4" s="2">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F4,'#venues'!$B$2:$B$15,0))</f>
+        <v>4</v>
+      </c>
+      <c r="H4" s="3">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F4,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="I4" s="2" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$D4,'#teams'!$B$2:$B$86,0))</f>
+        <v>mex</v>
+      </c>
+      <c r="J4" s="2" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$E4,'#teams'!$B$2:$B$86,0))</f>
+        <v>jam</v>
+      </c>
+      <c r="K4" s="2" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$I4,'#seeds'!$C$2:$C$17,0))</f>
+        <v>B1</v>
+      </c>
+      <c r="L4" s="2" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$J4,'#seeds'!$C$2:$C$17,0))</f>
+        <v>B4</v>
+      </c>
+      <c r="M4" s="18">
+        <f>'#matches'!$C4+'#matches'!$H4</f>
+        <v>45466.041666666672</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="7">
+        <v>45465.625</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="G5" s="5">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F5,'#venues'!$B$2:$B$15,0))</f>
+        <v>3</v>
+      </c>
+      <c r="H5" s="6">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F5,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="I5" s="5" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$D5,'#teams'!$B$2:$B$86,0))</f>
+        <v>ecu</v>
+      </c>
+      <c r="J5" s="5" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$E5,'#teams'!$B$2:$B$86,0))</f>
+        <v>ven</v>
+      </c>
+      <c r="K5" s="5" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$I5,'#seeds'!$C$2:$C$17,0))</f>
+        <v>B2</v>
+      </c>
+      <c r="L5" s="5" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$J5,'#seeds'!$C$2:$C$17,0))</f>
+        <v>B3</v>
+      </c>
+      <c r="M5" s="19">
+        <f>'#matches'!$C5+'#matches'!$H5</f>
+        <v>45465.916666666664</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="4">
+        <v>45466.708333333336</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="G6" s="2">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F6,'#venues'!$B$2:$B$15,0))</f>
+        <v>2</v>
+      </c>
+      <c r="H6" s="3">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F6,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="I6" s="2" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$D6,'#teams'!$B$2:$B$86,0))</f>
+        <v>usa</v>
+      </c>
+      <c r="J6" s="2" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$E6,'#teams'!$B$2:$B$86,0))</f>
+        <v>bol</v>
+      </c>
+      <c r="K6" s="2" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$I6,'#seeds'!$C$2:$C$17,0))</f>
+        <v>C1</v>
+      </c>
+      <c r="L6" s="2" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$J6,'#seeds'!$C$2:$C$17,0))</f>
+        <v>C4</v>
+      </c>
+      <c r="M6" s="18">
+        <f>'#matches'!$C6+'#matches'!$H6</f>
+        <v>45466.916666666672</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="7">
+        <v>45466.875</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="G7" s="5">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F7,'#venues'!$B$2:$B$15,0))</f>
+        <v>5</v>
+      </c>
+      <c r="H7" s="6">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F7,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I7" s="5" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$D7,'#teams'!$B$2:$B$86,0))</f>
+        <v>uru</v>
+      </c>
+      <c r="J7" s="5" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$E7,'#teams'!$B$2:$B$86,0))</f>
+        <v>pan</v>
+      </c>
+      <c r="K7" s="5" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$I7,'#seeds'!$C$2:$C$17,0))</f>
+        <v>C2</v>
+      </c>
+      <c r="L7" s="5" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$J7,'#seeds'!$C$2:$C$17,0))</f>
+        <v>C3</v>
+      </c>
+      <c r="M7" s="19">
+        <f>'#matches'!$C7+'#matches'!$H7</f>
+        <v>45467.041666666664</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="4">
+        <v>45467.75</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="G8" s="2">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F8,'#venues'!$B$2:$B$15,0))</f>
+        <v>6</v>
+      </c>
+      <c r="H8" s="3">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F8,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="I8" s="2" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$D8,'#teams'!$B$2:$B$86,0))</f>
+        <v>bra</v>
+      </c>
+      <c r="J8" s="2" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$E8,'#teams'!$B$2:$B$86,0))</f>
+        <v>crc</v>
+      </c>
+      <c r="K8" s="2" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$I8,'#seeds'!$C$2:$C$17,0))</f>
+        <v>D1</v>
+      </c>
+      <c r="L8" s="2" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$J8,'#seeds'!$C$2:$C$17,0))</f>
+        <v>D4</v>
+      </c>
+      <c r="M8" s="18">
+        <f>'#matches'!$C8+'#matches'!$H8</f>
+        <v>45468.041666666664</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C9" s="7">
+        <v>45467.708333333336</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="G9" s="5">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F9,'#venues'!$B$2:$B$15,0))</f>
+        <v>4</v>
+      </c>
+      <c r="H9" s="6">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F9,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="I9" s="5" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$D9,'#teams'!$B$2:$B$86,0))</f>
+        <v>col</v>
+      </c>
+      <c r="J9" s="5" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$E9,'#teams'!$B$2:$B$86,0))</f>
+        <v>par</v>
+      </c>
+      <c r="K9" s="5" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$I9,'#seeds'!$C$2:$C$17,0))</f>
+        <v>D2</v>
+      </c>
+      <c r="L9" s="5" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$J9,'#seeds'!$C$2:$C$17,0))</f>
+        <v>D3</v>
+      </c>
+      <c r="M9" s="19">
+        <f>'#matches'!$C9+'#matches'!$H9</f>
+        <v>45467.916666666672</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="4">
+        <v>45468.875</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="G10" s="2">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F10,'#venues'!$B$2:$B$15,0))</f>
+        <v>8</v>
+      </c>
+      <c r="H10" s="3">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F10,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I10" s="2" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$D10,'#teams'!$B$2:$B$86,0))</f>
+        <v>chi</v>
+      </c>
+      <c r="J10" s="2" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$E10,'#teams'!$B$2:$B$86,0))</f>
+        <v>arg</v>
+      </c>
+      <c r="K10" s="2" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$I10,'#seeds'!$C$2:$C$17,0))</f>
+        <v>A3</v>
+      </c>
+      <c r="L10" s="2" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$J10,'#seeds'!$C$2:$C$17,0))</f>
+        <v>A1</v>
+      </c>
+      <c r="M10" s="18">
+        <f>'#matches'!$C10+'#matches'!$H10</f>
+        <v>45469.041666666664</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="7">
+        <v>45468.708333333336</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="G11" s="5">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F11,'#venues'!$B$2:$B$15,0))</f>
+        <v>7</v>
+      </c>
+      <c r="H11" s="6">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F11,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="I11" s="5" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$D11,'#teams'!$B$2:$B$86,0))</f>
+        <v>per</v>
+      </c>
+      <c r="J11" s="5" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$E11,'#teams'!$B$2:$B$86,0))</f>
+        <v>can</v>
+      </c>
+      <c r="K11" s="5" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$I11,'#seeds'!$C$2:$C$17,0))</f>
+        <v>A2</v>
+      </c>
+      <c r="L11" s="5" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$J11,'#seeds'!$C$2:$C$17,0))</f>
+        <v>A4</v>
+      </c>
+      <c r="M11" s="19">
+        <f>'#matches'!$C11+'#matches'!$H11</f>
+        <v>45468.916666666672</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="4">
+        <v>45469.75</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="G12" s="2">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F12,'#venues'!$B$2:$B$15,0))</f>
+        <v>6</v>
+      </c>
+      <c r="H12" s="3">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F12,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="I12" s="2" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$D12,'#teams'!$B$2:$B$86,0))</f>
+        <v>ven</v>
+      </c>
+      <c r="J12" s="2" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$E12,'#teams'!$B$2:$B$86,0))</f>
+        <v>mex</v>
+      </c>
+      <c r="K12" s="2" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$I12,'#seeds'!$C$2:$C$17,0))</f>
+        <v>B3</v>
+      </c>
+      <c r="L12" s="2" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$J12,'#seeds'!$C$2:$C$17,0))</f>
+        <v>B1</v>
+      </c>
+      <c r="M12" s="18">
+        <f>'#matches'!$C12+'#matches'!$H12</f>
+        <v>45470.041666666664</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="7">
+        <v>45469.625</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="G13" s="5">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F13,'#venues'!$B$2:$B$15,0))</f>
+        <v>9</v>
+      </c>
+      <c r="H13" s="6">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F13,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="I13" s="5" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$D13,'#teams'!$B$2:$B$86,0))</f>
+        <v>ecu</v>
+      </c>
+      <c r="J13" s="5" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$E13,'#teams'!$B$2:$B$86,0))</f>
+        <v>jam</v>
+      </c>
+      <c r="K13" s="5" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$I13,'#seeds'!$C$2:$C$17,0))</f>
+        <v>B2</v>
+      </c>
+      <c r="L13" s="5" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$J13,'#seeds'!$C$2:$C$17,0))</f>
+        <v>B4</v>
+      </c>
+      <c r="M13" s="19">
+        <f>'#matches'!$C13+'#matches'!$H13</f>
+        <v>45469.916666666664</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="4">
+        <v>45470.75</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="G14" s="2">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F14,'#venues'!$B$2:$B$15,0))</f>
+        <v>1</v>
+      </c>
+      <c r="H14" s="3">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F14,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I14" s="2" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$D14,'#teams'!$B$2:$B$86,0))</f>
+        <v>pan</v>
+      </c>
+      <c r="J14" s="2" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$E14,'#teams'!$B$2:$B$86,0))</f>
+        <v>usa</v>
+      </c>
+      <c r="K14" s="2" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$I14,'#seeds'!$C$2:$C$17,0))</f>
+        <v>C3</v>
+      </c>
+      <c r="L14" s="2" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$J14,'#seeds'!$C$2:$C$17,0))</f>
+        <v>C1</v>
+      </c>
+      <c r="M14" s="18">
+        <f>'#matches'!$C14+'#matches'!$H14</f>
+        <v>45470.916666666664</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="7">
+        <v>45470.875</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="G15" s="5">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F15,'#venues'!$B$2:$B$15,0))</f>
+        <v>8</v>
+      </c>
+      <c r="H15" s="6">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F15,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I15" s="5" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$D15,'#teams'!$B$2:$B$86,0))</f>
+        <v>uru</v>
+      </c>
+      <c r="J15" s="5" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$E15,'#teams'!$B$2:$B$86,0))</f>
+        <v>bol</v>
+      </c>
+      <c r="K15" s="5" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$I15,'#seeds'!$C$2:$C$17,0))</f>
+        <v>C2</v>
+      </c>
+      <c r="L15" s="5" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$J15,'#seeds'!$C$2:$C$17,0))</f>
+        <v>C4</v>
+      </c>
+      <c r="M15" s="19">
+        <f>'#matches'!$C15+'#matches'!$H15</f>
+        <v>45471.041666666664</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="4">
+        <v>45471.75</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G16" s="2">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F16,'#venues'!$B$2:$B$15,0))</f>
+        <v>9</v>
+      </c>
+      <c r="H16" s="3">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F16,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="I16" s="2" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$D16,'#teams'!$B$2:$B$86,0))</f>
+        <v>par</v>
+      </c>
+      <c r="J16" s="2" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$E16,'#teams'!$B$2:$B$86,0))</f>
+        <v>bra</v>
+      </c>
+      <c r="K16" s="2" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$I16,'#seeds'!$C$2:$C$17,0))</f>
+        <v>D3</v>
+      </c>
+      <c r="L16" s="2" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$J16,'#seeds'!$C$2:$C$17,0))</f>
+        <v>D1</v>
+      </c>
+      <c r="M16" s="18">
+        <f>'#matches'!$C16+'#matches'!$H16</f>
+        <v>45472.041666666664</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="7">
+        <v>45471.625</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="G17" s="5">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F17,'#venues'!$B$2:$B$15,0))</f>
+        <v>10</v>
+      </c>
+      <c r="H17" s="6">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F17,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="I17" s="5" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$D17,'#teams'!$B$2:$B$86,0))</f>
+        <v>col</v>
+      </c>
+      <c r="J17" s="5" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$E17,'#teams'!$B$2:$B$86,0))</f>
+        <v>crc</v>
+      </c>
+      <c r="K17" s="5" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$I17,'#seeds'!$C$2:$C$17,0))</f>
+        <v>D2</v>
+      </c>
+      <c r="L17" s="5" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$J17,'#seeds'!$C$2:$C$17,0))</f>
+        <v>D4</v>
+      </c>
+      <c r="M17" s="19">
+        <f>'#matches'!$C17+'#matches'!$H17</f>
+        <v>45471.916666666664</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="4">
+        <v>45472.833333333336</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G18" s="2">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F18,'#venues'!$B$2:$B$15,0))</f>
+        <v>5</v>
+      </c>
+      <c r="H18" s="3">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F18,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I18" s="2" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$D18,'#teams'!$B$2:$B$86,0))</f>
+        <v>arg</v>
+      </c>
+      <c r="J18" s="2" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$E18,'#teams'!$B$2:$B$86,0))</f>
+        <v>per</v>
+      </c>
+      <c r="K18" s="2" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$I18,'#seeds'!$C$2:$C$17,0))</f>
+        <v>A1</v>
+      </c>
+      <c r="L18" s="2" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$J18,'#seeds'!$C$2:$C$17,0))</f>
+        <v>A2</v>
+      </c>
+      <c r="M18" s="18">
+        <f>'#matches'!$C18+'#matches'!$H18</f>
+        <v>45473</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="7">
+        <v>45472.833333333336</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="G19" s="5">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F19,'#venues'!$B$2:$B$15,0))</f>
+        <v>11</v>
+      </c>
+      <c r="H19" s="6">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F19,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I19" s="5" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$D19,'#teams'!$B$2:$B$86,0))</f>
+        <v>can</v>
+      </c>
+      <c r="J19" s="5" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$E19,'#teams'!$B$2:$B$86,0))</f>
+        <v>chi</v>
+      </c>
+      <c r="K19" s="5" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$I19,'#seeds'!$C$2:$C$17,0))</f>
+        <v>A4</v>
+      </c>
+      <c r="L19" s="5" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$J19,'#seeds'!$C$2:$C$17,0))</f>
+        <v>A3</v>
+      </c>
+      <c r="M19" s="19">
+        <f>'#matches'!$C19+'#matches'!$H19</f>
+        <v>45473</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="4">
+        <v>45473.708333333336</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G20" s="2">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F20,'#venues'!$B$2:$B$15,0))</f>
+        <v>10</v>
+      </c>
+      <c r="H20" s="3">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F20,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="I20" s="2" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$D20,'#teams'!$B$2:$B$86,0))</f>
+        <v>mex</v>
+      </c>
+      <c r="J20" s="2" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$E20,'#teams'!$B$2:$B$86,0))</f>
+        <v>ecu</v>
+      </c>
+      <c r="K20" s="2" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$I20,'#seeds'!$C$2:$C$17,0))</f>
+        <v>B1</v>
+      </c>
+      <c r="L20" s="2" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$J20,'#seeds'!$C$2:$C$17,0))</f>
+        <v>B2</v>
+      </c>
+      <c r="M20" s="18">
+        <f>'#matches'!$C20+'#matches'!$H20</f>
+        <v>45474</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="7">
+        <v>45473.791666666664</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G21" s="5">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F21,'#venues'!$B$2:$B$15,0))</f>
+        <v>12</v>
+      </c>
+      <c r="H21" s="6">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F21,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="I21" s="5" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$D21,'#teams'!$B$2:$B$86,0))</f>
+        <v>jam</v>
+      </c>
+      <c r="J21" s="5" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$E21,'#teams'!$B$2:$B$86,0))</f>
+        <v>ven</v>
+      </c>
+      <c r="K21" s="5" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$I21,'#seeds'!$C$2:$C$17,0))</f>
+        <v>B4</v>
+      </c>
+      <c r="L21" s="5" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$J21,'#seeds'!$C$2:$C$17,0))</f>
+        <v>B3</v>
+      </c>
+      <c r="M21" s="19">
+        <f>'#matches'!$C21+'#matches'!$H21</f>
+        <v>45474</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="4">
+        <v>45474.833333333336</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="G22" s="2">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F22,'#venues'!$B$2:$B$15,0))</f>
+        <v>13</v>
+      </c>
+      <c r="H22" s="3">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F22,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="I22" s="2" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$D22,'#teams'!$B$2:$B$86,0))</f>
+        <v>usa</v>
+      </c>
+      <c r="J22" s="2" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$E22,'#teams'!$B$2:$B$86,0))</f>
+        <v>uru</v>
+      </c>
+      <c r="K22" s="2" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$I22,'#seeds'!$C$2:$C$17,0))</f>
+        <v>C1</v>
+      </c>
+      <c r="L22" s="2" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$J22,'#seeds'!$C$2:$C$17,0))</f>
+        <v>C2</v>
+      </c>
+      <c r="M22" s="18">
+        <f>'#matches'!$C22+'#matches'!$H22</f>
+        <v>45475.041666666672</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="7">
+        <v>45474.875</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="G23" s="5">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F23,'#venues'!$B$2:$B$15,0))</f>
+        <v>11</v>
+      </c>
+      <c r="H23" s="6">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F23,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I23" s="5" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$D23,'#teams'!$B$2:$B$86,0))</f>
+        <v>bol</v>
+      </c>
+      <c r="J23" s="5" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$E23,'#teams'!$B$2:$B$86,0))</f>
+        <v>pan</v>
+      </c>
+      <c r="K23" s="5" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$I23,'#seeds'!$C$2:$C$17,0))</f>
+        <v>C4</v>
+      </c>
+      <c r="L23" s="5" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$J23,'#seeds'!$C$2:$C$17,0))</f>
+        <v>C3</v>
+      </c>
+      <c r="M23" s="19">
+        <f>'#matches'!$C23+'#matches'!$H23</f>
+        <v>45475.041666666664</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="4">
+        <v>45475.75</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="G24" s="2">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F24,'#venues'!$B$2:$B$15,0))</f>
+        <v>3</v>
+      </c>
+      <c r="H24" s="3">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F24,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="I24" s="2" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$D24,'#teams'!$B$2:$B$86,0))</f>
+        <v>bra</v>
+      </c>
+      <c r="J24" s="2" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$E24,'#teams'!$B$2:$B$86,0))</f>
+        <v>col</v>
+      </c>
+      <c r="K24" s="2" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$I24,'#seeds'!$C$2:$C$17,0))</f>
+        <v>D1</v>
+      </c>
+      <c r="L24" s="2" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$J24,'#seeds'!$C$2:$C$17,0))</f>
+        <v>D2</v>
+      </c>
+      <c r="M24" s="18">
+        <f>'#matches'!$C24+'#matches'!$H24</f>
+        <v>45476.041666666664</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="7">
+        <v>45475.833333333336</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G25" s="5">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F25,'#venues'!$B$2:$B$15,0))</f>
+        <v>12</v>
+      </c>
+      <c r="H25" s="6">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F25,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="I25" s="5" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$D25,'#teams'!$B$2:$B$86,0))</f>
+        <v>crc</v>
+      </c>
+      <c r="J25" s="5" t="str">
+        <f>INDEX('#teams'!$A$2:$A$86,MATCH('#matches'!$E25,'#teams'!$B$2:$B$86,0))</f>
+        <v>par</v>
+      </c>
+      <c r="K25" s="5" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$I25,'#seeds'!$C$2:$C$17,0))</f>
+        <v>D4</v>
+      </c>
+      <c r="L25" s="5" t="str">
+        <f>INDEX('#seeds'!$A$2:$A$17,MATCH('#matches'!$J25,'#seeds'!$C$2:$C$17,0))</f>
+        <v>D3</v>
+      </c>
+      <c r="M25" s="19">
+        <f>'#matches'!$C25+'#matches'!$H25</f>
+        <v>45476.041666666672</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C26" s="4">
+        <v>45477.833333333336</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G26" s="2">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F26,'#venues'!$B$2:$B$15,0))</f>
+        <v>4</v>
+      </c>
+      <c r="H26" s="3">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F26,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M26" s="18">
+        <f>'#matches'!$C26+'#matches'!$H26</f>
+        <v>45478.041666666672</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A27" s="5">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="7">
+        <v>45478.833333333336</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="G27" s="5">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F27,'#venues'!$B$2:$B$15,0))</f>
+        <v>2</v>
+      </c>
+      <c r="H27" s="6">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F27,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M27" s="19">
+        <f>'#matches'!$C27+'#matches'!$H27</f>
+        <v>45479.041666666672</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="4">
+        <v>45479.75</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G28" s="2">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F28,'#venues'!$B$2:$B$15,0))</f>
+        <v>9</v>
+      </c>
+      <c r="H28" s="3">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F28,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M28" s="18">
+        <f>'#matches'!$C28+'#matches'!$H28</f>
+        <v>45480.041666666664</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A29" s="5">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="7">
+        <v>45479.625</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="G29" s="5">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F29,'#venues'!$B$2:$B$15,0))</f>
+        <v>10</v>
+      </c>
+      <c r="H29" s="6">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F29,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M29" s="19">
+        <f>'#matches'!$C29+'#matches'!$H29</f>
+        <v>45479.916666666664</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C30" s="4">
+        <v>45482.833333333336</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="G30" s="2">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F30,'#venues'!$B$2:$B$15,0))</f>
+        <v>8</v>
+      </c>
+      <c r="H30" s="3">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F30,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="M30" s="18">
+        <f>'#matches'!$C30+'#matches'!$H30</f>
+        <v>45483</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A31" s="5">
+        <v>30</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="7">
+        <v>45483.833333333336</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="G31" s="5">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F31,'#venues'!$B$2:$B$15,0))</f>
+        <v>14</v>
+      </c>
+      <c r="H31" s="6">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F31,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="L31" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="M31" s="19">
+        <f>'#matches'!$C31+'#matches'!$H31</f>
+        <v>45484</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C32" s="4">
+        <v>45486.833333333336</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G32" s="2">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F32,'#venues'!$B$2:$B$15,0))</f>
+        <v>14</v>
+      </c>
+      <c r="H32" s="3">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F32,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="M32" s="18">
+        <f>'#matches'!$C32+'#matches'!$H32</f>
+        <v>45487</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A33" s="5">
+        <v>32</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C33" s="7">
+        <v>45487.833333333336</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="G33" s="5">
+        <f>INDEX('#venues'!$A$2:$A$15,MATCH('#matches'!$F33,'#venues'!$B$2:$B$15,0))</f>
+        <v>5</v>
+      </c>
+      <c r="H33" s="6">
+        <f>INDEX('#venues'!$C$2:$C$15,MATCH('#matches'!$F33,'#venues'!$B$2:$B$15,0))</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="L33" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="M33" s="19">
+        <f>'#matches'!$C33+'#matches'!$H33</f>
+        <v>45488</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I1" r:id="rId1" xr:uid="{563C6176-72B2-487F-9616-1231C7EAB1DE}"/>
+    <hyperlink ref="K1" r:id="rId2" xr:uid="{3AC78D15-5944-44DC-9B61-49E1E20B05D5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{593E01A1-36F9-4165-B8E7-F35B40188BA9}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.7" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="3" max="3" width="11.9375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A1" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="2" t="str">
+        <f>LOWER('#seeds'!$B2)</f>
+        <v>arg</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <f>LOWER('#seeds'!$B3)</f>
+        <v>per</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="2" t="str">
+        <f>LOWER('#seeds'!$B4)</f>
+        <v>chi</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="5" t="str">
+        <f>LOWER('#seeds'!$B5)</f>
+        <v>can</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="2" t="str">
+        <f>LOWER('#seeds'!$B6)</f>
+        <v>mex</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="5" t="str">
+        <f>LOWER('#seeds'!$B7)</f>
+        <v>ecu</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="2" t="str">
+        <f>LOWER('#seeds'!$B8)</f>
+        <v>ven</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="5" t="str">
+        <f>LOWER('#seeds'!$B9)</f>
+        <v>jam</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="2" t="str">
+        <f>LOWER('#seeds'!$B10)</f>
+        <v>usa</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="5" t="str">
+        <f>LOWER('#seeds'!$B11)</f>
+        <v>uru</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="2" t="str">
+        <f>LOWER('#seeds'!$B12)</f>
+        <v>pan</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="5" t="str">
+        <f>LOWER('#seeds'!$B13)</f>
+        <v>bol</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="2" t="str">
+        <f>LOWER('#seeds'!$B14)</f>
+        <v>bra</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="5" t="str">
+        <f>LOWER('#seeds'!$B15)</f>
+        <v>col</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="2" t="str">
+        <f>LOWER('#seeds'!$B16)</f>
+        <v>par</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="5" t="str">
+        <f>LOWER('#seeds'!$B17)</f>
+        <v>crc</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF7C20BB-FC56-412B-823F-DE72033ECE98}">
+  <dimension ref="A1:B86"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B86"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.7" x14ac:dyDescent="0.5"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A1" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A2" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A3" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A4" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A5" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A6" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A7" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A8" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A9" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A10" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A11" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A12" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A13" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A14" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A15" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A16" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A17" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A18" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A19" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A20" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A21" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A22" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A23" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A24" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A25" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A26" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A27" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A28" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A29" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A30" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A31" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A32" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A33" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A34" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A35" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A36" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A37" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A38" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A39" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A40" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A41" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A42" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A43" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A44" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A45" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A46" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A47" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A48" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A49" s="5" t="s">
+        <v>320</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A50" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A51" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A52" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A53" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A54" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A55" s="5" t="s">
+        <v>308</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A56" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A57" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A58" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A59" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A60" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A61" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A62" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A63" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A64" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A65" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A66" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A67" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A68" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A69" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A70" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A71" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A72" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A73" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A74" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A75" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A76" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A77" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A78" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A79" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A80" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A81" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A82" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A83" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B83" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A84" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A85" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A86" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA0D500E-A934-4555-A8FD-A3A34D26AF2C}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.7" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="12.703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5859375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.9375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A1" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>404</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" s="12">
+        <f>TIME(4,0,0)</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="C3" s="10">
+        <f>TIME(5,0,0)</f>
+        <v>0.20833333333333334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="C4" s="8">
+        <f>TIME(7,0,0)</f>
+        <v>0.29166666666666669</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="C5" s="10">
+        <f>TIME(5,0,0)</f>
+        <v>0.20833333333333334</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="C6" s="8">
+        <f>TIME(4,0,0)</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="C7" s="10">
+        <f>TIME(7,0,0)</f>
+        <v>0.29166666666666669</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="C8" s="8">
+        <f>TIME(5,0,0)</f>
+        <v>0.20833333333333334</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A9" s="11">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="C9" s="10">
+        <f>TIME(4,0,0)</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A10" s="9">
+        <v>9</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="C10" s="8">
+        <f>TIME(7,0,0)</f>
+        <v>0.29166666666666669</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A11" s="11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C11" s="10">
+        <f>TIME(7,0,0)</f>
+        <v>0.29166666666666669</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A12" s="9">
+        <v>11</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C12" s="8">
+        <f>TIME(4,0,0)</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A13" s="11">
+        <v>12</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="C13" s="10">
+        <f>TIME(5,0,0)</f>
+        <v>0.20833333333333334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A14" s="9">
+        <v>13</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C14" s="8">
+        <f>TIME(5,0,0)</f>
+        <v>0.20833333333333334</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A15" s="23">
+        <v>14</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="C15" s="24">
+        <f>TIME(4,0,0)</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{331DF06F-5385-4C45-B7C5-E682A6319987}">
+  <dimension ref="A1:I25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.7" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="2" max="2" width="9.46875" customWidth="1"/>
+    <col min="8" max="8" width="16.52734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A1" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="D1" t="str" cm="1">
+        <f t="array" ref="D1:D14">_xlfn.UNIQUE(A1:A25)</f>
+        <v>Atlanta, GA (Mercedes-Benz Stadium)</v>
+      </c>
+      <c r="H1" t="str" cm="1">
+        <f t="array" ref="H1:I1">_xlfn.TEXTSPLIT(D1, " (")</f>
+        <v>Atlanta, GA</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Mercedes-Benz Stadium)</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A2" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Arlington, TX (AT&amp;T Stadium)</v>
+      </c>
+      <c r="H2" t="str" cm="1">
+        <f t="array" ref="H2:I2">_xlfn.TEXTSPLIT(D2, " (")</f>
+        <v>Arlington, TX</v>
+      </c>
+      <c r="I2" t="str">
+        <v>AT&amp;T Stadium)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A3" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Santa Clara, CA (Levi's Stadium)</v>
+      </c>
+      <c r="H3" t="str" cm="1">
+        <f t="array" ref="H3:I3">_xlfn.TEXTSPLIT(D3, " (")</f>
+        <v>Santa Clara, CA</v>
+      </c>
+      <c r="I3" t="str">
+        <v>Levi's Stadium)</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A4" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Houston, TX (NRG Stadium)</v>
+      </c>
+      <c r="H4" t="str" cm="1">
+        <f t="array" ref="H4:I4">_xlfn.TEXTSPLIT(D4, " (")</f>
+        <v>Houston, TX</v>
+      </c>
+      <c r="I4" t="str">
+        <v>NRG Stadium)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A5" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Miami, FL (Hard Rock Stadium)</v>
+      </c>
+      <c r="H5" t="str" cm="1">
+        <f t="array" ref="H5:I5">_xlfn.TEXTSPLIT(D5, " (")</f>
+        <v>Miami, FL</v>
+      </c>
+      <c r="I5" t="str">
+        <v>Hard Rock Stadium)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A6" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Inglewood, CA (SoFi Stadium)</v>
+      </c>
+      <c r="H6" t="str" cm="1">
+        <f t="array" ref="H6:I6">_xlfn.TEXTSPLIT(D6, " (")</f>
+        <v>Inglewood, CA</v>
+      </c>
+      <c r="I6" t="str">
+        <v>SoFi Stadium)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A7" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Kansas City, KS (Children's Mercy Park)</v>
+      </c>
+      <c r="H7" t="str" cm="1">
+        <f t="array" ref="H7:I7">_xlfn.TEXTSPLIT(D7, " (")</f>
+        <v>Kansas City, KS</v>
+      </c>
+      <c r="I7" t="str">
+        <v>Children's Mercy Park)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A8" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="D8" t="str">
+        <v>East Rutherford, NJ (MetLife Stadium)</v>
+      </c>
+      <c r="H8" t="str" cm="1">
+        <f t="array" ref="H8:I8">_xlfn.TEXTSPLIT(D8, " (")</f>
+        <v>East Rutherford, NJ</v>
+      </c>
+      <c r="I8" t="str">
+        <v>MetLife Stadium)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A9" s="16" t="s">
+        <v>237</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Las Vegas, NV (Allegiant Stadium)</v>
+      </c>
+      <c r="H9" t="str" cm="1">
+        <f t="array" ref="H9:I9">_xlfn.TEXTSPLIT(D9, " (")</f>
+        <v>Las Vegas, NV</v>
+      </c>
+      <c r="I9" t="str">
+        <v>Allegiant Stadium)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A10" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Glendale, AZ (State Farm Stadium)</v>
+      </c>
+      <c r="H10" t="str" cm="1">
+        <f t="array" ref="H10:I10">_xlfn.TEXTSPLIT(D10, " (")</f>
+        <v>Glendale, AZ</v>
+      </c>
+      <c r="I10" t="str">
+        <v>State Farm Stadium)</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A11" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Orlando, FL (Exploria Stadium)</v>
+      </c>
+      <c r="H11" t="str" cm="1">
+        <f t="array" ref="H11:I11">_xlfn.TEXTSPLIT(D11, " (")</f>
+        <v>Orlando, FL</v>
+      </c>
+      <c r="I11" t="str">
+        <v>Exploria Stadium)</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A12" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Austin, TX (Q2 Stadium)</v>
+      </c>
+      <c r="H12" t="str" cm="1">
+        <f t="array" ref="H12:I12">_xlfn.TEXTSPLIT(D12, " (")</f>
+        <v>Austin, TX</v>
+      </c>
+      <c r="I12" t="str">
+        <v>Q2 Stadium)</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A13" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="D13" t="str">
+        <v>Kansas City, MO (Arrowhead Stadium)</v>
+      </c>
+      <c r="H13" t="str" cm="1">
+        <f t="array" ref="H13:I13">_xlfn.TEXTSPLIT(D13, " (")</f>
+        <v>Kansas City, MO</v>
+      </c>
+      <c r="I13" t="str">
+        <v>Arrowhead Stadium)</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A14" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="D14" t="str">
+        <v>Charlotte, NC (Bank of America Stadium)</v>
+      </c>
+      <c r="H14" t="str" cm="1">
+        <f t="array" ref="H14:I14">_xlfn.TEXTSPLIT(D14, " (")</f>
+        <v>Charlotte, NC</v>
+      </c>
+      <c r="I14" t="str">
+        <v>Bank of America Stadium)</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A15" s="16" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A16" s="15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A17" s="16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A18" s="15" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A19" s="16" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A20" s="15" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A21" s="16" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A22" s="15" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A23" s="16" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A24" s="15" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="14.35" x14ac:dyDescent="0.5">
+      <c r="A25" s="14" t="s">
+        <v>193</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>